<commit_message>
refactoring to handle reporting and two known types of inventory
</commit_message>
<xml_diff>
--- a/dell/invent.xml_report.xlsx
+++ b/dell/invent.xml_report.xlsx
@@ -14,23 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
-  <si>
-    <t>ServiceTag</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
+  <si>
+    <t>data</t>
   </si>
   <si>
     <t>C1WN2S2</t>
   </si>
   <si>
-    <t>CPU model</t>
-  </si>
-  <si>
     <t>Intel(R) Xeon(R) CPU E5-2630 v4 @ 2.20GHz</t>
   </si>
   <si>
-    <t>PCI device</t>
-  </si>
-  <si>
     <t>PERC H730P Mini</t>
   </si>
   <si>
@@ -85,15 +79,9 @@
     <t>C610/X99 series chipset PCI Express Root Port #8</t>
   </si>
   <si>
-    <t>System memory size</t>
-  </si>
-  <si>
     <t>262144</t>
   </si>
   <si>
-    <t>Memory serial</t>
-  </si>
-  <si>
     <t>2CCA2D56</t>
   </si>
   <si>
@@ -118,15 +106,9 @@
     <t>2CCA2DCF</t>
   </si>
   <si>
-    <t>Memory module part number</t>
-  </si>
-  <si>
     <t>HMA84GR7AFR4N-UH</t>
   </si>
   <si>
-    <t>Memory slot</t>
-  </si>
-  <si>
     <t>DIMM.Socket.A1</t>
   </si>
   <si>
@@ -151,9 +133,6 @@
     <t>DIMM.Socket.B4</t>
   </si>
   <si>
-    <t>HDD serial</t>
-  </si>
-  <si>
     <t>WFK1QAS1</t>
   </si>
   <si>
@@ -178,21 +157,12 @@
     <t>WFK1Q9VX</t>
   </si>
   <si>
-    <t>HDD model</t>
-  </si>
-  <si>
     <t>ST1200MM0099</t>
   </si>
   <si>
-    <t>HDD fw</t>
-  </si>
-  <si>
     <t>ST31</t>
   </si>
   <si>
-    <t>HDD slot population</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -217,28 +187,16 @@
     <t>7</t>
   </si>
   <si>
-    <t>PSU part number</t>
-  </si>
-  <si>
     <t>05RHVVA02</t>
   </si>
   <si>
-    <t>PSU serial</t>
-  </si>
-  <si>
     <t>CNDED0088K96MB</t>
   </si>
   <si>
     <t>CNDED0088K96P6</t>
   </si>
   <si>
-    <t>PSU model</t>
-  </si>
-  <si>
     <t xml:space="preserve">PWR SPLY,750W,RDNT,DELTA      </t>
-  </si>
-  <si>
-    <t>PSU fw</t>
   </si>
   <si>
     <t>00.24.7D</t>
@@ -579,18 +537,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
     <col min="2" max="2" width="41.7109375" customWidth="1"/>
     <col min="3" max="3" width="63.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
     <col min="13" max="13" width="14.7109375" customWidth="1"/>
     <col min="14" max="14" width="30.7109375" customWidth="1"/>
     <col min="15" max="15" width="8.7109375" customWidth="1"/>
@@ -601,46 +559,46 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="J1" t="s">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="K1" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="L1" t="s">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="M1" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="N1" t="s">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="O1" t="s">
-        <v>74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -648,313 +606,313 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" t="s">
         <v>57</v>
       </c>
-      <c r="K2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" t="s">
-        <v>68</v>
-      </c>
       <c r="M2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N2" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="O2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
         <v>47</v>
       </c>
-      <c r="I3" t="s">
-        <v>55</v>
-      </c>
       <c r="J3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" t="s">
         <v>57</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" t="s">
         <v>60</v>
       </c>
-      <c r="L3" t="s">
-        <v>68</v>
-      </c>
-      <c r="M3" t="s">
-        <v>71</v>
-      </c>
-      <c r="N3" t="s">
-        <v>73</v>
-      </c>
       <c r="O3" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" t="s">
         <v>48</v>
       </c>
-      <c r="I4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" t="s">
-        <v>57</v>
-      </c>
       <c r="K4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="J5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="C6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
         <v>30</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>35</v>
       </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
       <c r="H6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K6" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="C7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="I7" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="J7" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K7" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="C8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H8" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" t="s">
         <v>55</v>
-      </c>
-      <c r="J8" t="s">
-        <v>57</v>
-      </c>
-      <c r="K8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="C9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="J9" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K9" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="C10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="C11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="C12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="C13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="C14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="C15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="C16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="3:3">
       <c r="C21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="3:3">
       <c r="C23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added per component comparsion
</commit_message>
<xml_diff>
--- a/dell/invent.xml_report.xlsx
+++ b/dell/invent.xml_report.xlsx
@@ -19,7 +19,7 @@
     <t>ServiceTag</t>
   </si>
   <si>
-    <t>C1WN2S2</t>
+    <t>['C1WN2S2']</t>
   </si>
   <si>
     <t>CPU model</t>
@@ -88,7 +88,7 @@
     <t>System memory size</t>
   </si>
   <si>
-    <t>262144</t>
+    <t>['262144']</t>
   </si>
   <si>
     <t>Memory serial</t>

</xml_diff>

<commit_message>
comments with golden configuration
</commit_message>
<xml_diff>
--- a/dell/invent.xml_report.xlsx
+++ b/dell/invent.xml_report.xlsx
@@ -13,6 +13,770 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Intel(R) Xeon(R) CPU E5-2630 v4 @ 2.20GHz not equal golden setting Intel(R) Xeon(R) CPU E5-2620 v3 @ 2.40GHz </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">PERC H730P Mini not equal golden setting C610/X99 series chipset sSATA Controller [AHCI mode] </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">262144 not equal golden setting 65536 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">HMA84GR7AFR4N-UH not equal golden setting M393A1G43DB0-CPB </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST1200MM0099 not equal golden setting ST300MM0008 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST31 not equal golden setting TT31 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">05RHVVA02 not equal golden setting 0V1YJ6A00 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">00.24.7D not equal golden setting 00.24.71 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Intel(R) Xeon(R) CPU E5-2630 v4 @ 2.20GHz not equal golden setting Intel(R) Xeon(R) CPU E5-2620 v3 @ 2.40GHz </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Ethernet 10G 4P X520/I350 rNDC not equal golden setting C610/X99 series chipset 6-Port SATA Controller [AHCI mode] </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">HMA84GR7AFR4N-UH not equal golden setting M393A1G43DB0-CPB </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST1200MM0099 not equal golden setting ST300MM0008 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST31 not equal golden setting TT31 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">05RHVVA02 not equal golden setting 0V1YJ6A00 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">00.24.7D not equal golden setting 00.24.71 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Ethernet 10G 4P X520/I350 rNDC not equal golden setting ISP2532-based 8Gb Fibre Channel to PCI Express HBA </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">HMA84GR7AFR4N-UH not equal golden setting M393A1G43DB0-CPB </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST1200MM0099 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST31 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">2 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">I350 Gigabit Network Connection not equal golden setting ISP2532-based 8Gb Fibre Channel to PCI Express HBA </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">HMA84GR7AFR4N-UH not equal golden setting M393A1G43DB0-CPB </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST1200MM0099 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST31 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">3 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">I350 Gigabit Network Connection not equal golden setting Terminator 2x/i </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">HMA84GR7AFR4N-UH not equal golden setting M393A1G43DB0-CPB </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST1200MM0099 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST31 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">4 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">G200eR2 not equal golden setting C610/X99 series chipset LPC Controller </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">HMA84GR7AFR4N-UH not equal golden setting M393A1G43DB0-CPB </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST1200MM0099 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST31 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">5 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">C610/X99 series chipset sSATA Controller [AHCI mode] not equal golden setting Ethernet 10G 4P X520/I350 rNDC </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">HMA84GR7AFR4N-UH not equal golden setting M393A1G43DB0-CPB </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST1200MM0099 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST31 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">6 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Xeon E7 v4/Xeon E5 v4/Xeon E3 v4/Xeon D DMI2 not equal golden setting Ethernet 10G 4P X520/I350 rNDC </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">HMA84GR7AFR4N-UH not equal golden setting M393A1G43DB0-CPB </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST1200MM0099 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST31 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">7 not equal golden setting not availalable in master configuration </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">SH7758 PCIe Switch [PS] not equal golden setting I350 Gigabit Network Connection </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">C610/X99 series chipset USB Enhanced Host Controller #1 not equal golden setting I350 Gigabit Network Connection </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">C610/X99 series chipset LPC Controller not equal golden setting Renesas Technology Corp. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">C610/X99 series chipset 6-Port SATA Controller [AHCI mode] not equal golden setting Terminator 2x/i </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Xeon E7 v4/Xeon E5 v4/Xeon E3 v4/Xeon D PCI Express Root Port 1 not equal golden setting Renesas Technology Corp. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">C610/X99 series chipset USB Enhanced Host Controller #2 not equal golden setting Renesas Technology Corp. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">SH7758 PCIe Switch [PS] not equal golden setting Terminator 2x/i </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Xeon E7 v4/Xeon E5 v4/Xeon E3 v4/Xeon D PCI Express Root Port 2 not equal golden setting Renesas Technology Corp. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">SH7758 PCIe-PCI Bridge [PPB] not equal golden setting C610/X99 series chipset PCI Express Root Port #1 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Xeon E7 v4/Xeon E5 v4/Xeon E3 v4/Xeon D PCI Express Root Port 3 not equal golden setting Terminator 2x/i </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">C610/X99 series chipset PCI Express Root Port #1 not equal golden setting C610/X99 series chipset PCI Express Root Port #8 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">C610/X99 series chipset PCI Express Root Port #8 not equal golden setting PERC H330 Mini </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">SH7758 PCIe Switch [PS] not equal golden setting C610/X99 series chipset USB Enhanced Host Controller #1 </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="38">
   <si>
@@ -134,13 +898,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -192,12 +962,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,373 +1288,374 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="J2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="2" t="s">
+      <c r="M2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" s="4" t="s">
+      <c r="J3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N3" s="2" t="s">
+      <c r="M3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="G4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="J4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="D5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="G5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="J5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="D6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="4" t="s">
+      <c r="G6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L6" s="3" t="s">
+      <c r="J6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="D7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="4" t="s">
+      <c r="G7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L7" s="3" t="s">
+      <c r="J7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="D8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="D8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="G8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L8" s="3" t="s">
+      <c r="J8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="D9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="D9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="G9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L9" s="3" t="s">
+      <c r="J9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:16">
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="4:4">
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="4:4">
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="4:4">
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="4:4">
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="4:4">
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="4:4">
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="4:4">
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="4" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>